<commit_message>
Added Testcases for the Sprint#2 Screens
</commit_message>
<xml_diff>
--- a/TestCases_Catalog/Catalog-Tool.xlsx
+++ b/TestCases_Catalog/Catalog-Tool.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagadeesh/Documents/Testing/TestCases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagadeesh/Documents/Development_Workspace/commerce-ui/TestCases_Catalog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC589E08-D23D-B149-99E1-4252CD79767A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78B6298D-4890-414A-A881-7667B7160E9D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14240" xr2:uid="{9945D0DC-294A-F34F-AE9E-0AF1EF0B8DAB}"/>
   </bookViews>
@@ -23,7 +23,10 @@
     <sheet name="References" sheetId="8" r:id="rId8"/>
     <sheet name="Search Results" sheetId="9" r:id="rId9"/>
     <sheet name="Unassigned Catalog Entries" sheetId="10" r:id="rId10"/>
-    <sheet name="Extended sites store sales cata" sheetId="11" r:id="rId11"/>
+    <sheet name="Catalog Uploads" sheetId="13" r:id="rId11"/>
+    <sheet name="Selecting Store" sheetId="14" r:id="rId12"/>
+    <sheet name="Extended Sites Catalog Asset St" sheetId="15" r:id="rId13"/>
+    <sheet name="Extended sites store sales cata" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="436">
   <si>
     <t>Objective</t>
   </si>
@@ -1986,6 +1989,461 @@
     <t>Need to Write test cases how to get or add Content on the page
 Comment: 
 I have no idea , need to explore about the same</t>
+  </si>
+  <si>
+    <t>From the File menu , selecting the Catalog Upload   screen</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option</t>
+  </si>
+  <si>
+    <t>System should display the  New catalog upload screen with Manage catalog upload options consist
+-Main Properties
+File Name 
+Size
+Character
+Target Catalog</t>
+  </si>
+  <si>
+    <t>Browse and File upload through File Name field</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option</t>
+  </si>
+  <si>
+    <t>System should display new pop up window to browse and select the CSV or XML files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File selection from the popup window </t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the CSV File and cilck on Choose Button</t>
+  </si>
+  <si>
+    <t>System should allow to select the CSV fil e and once clicked on Choose Button it should be selected successfully .</t>
+  </si>
+  <si>
+    <t>File selection from the popup window and check the size of the selected file in the SIZE field</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the CSV File and cilck on Choose Button
+8.Check the file size in the SIZE field</t>
+  </si>
+  <si>
+    <t>System should display the Size in KB format once uploaded the file .</t>
+  </si>
+  <si>
+    <t>File selection from the popup window for XML file format</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML File and cilck on Choose Button</t>
+  </si>
+  <si>
+    <t>System should allow to select the XML file and once clicked on Choose Button it should be selected successfully .</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML File and cilck on Choose Button
+8.Check the file size in the SIZE field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecting the Character set to catalog upload </t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+     UTF-8
+     UTF-16
+    GB2312
+    Big5
+    Windows Latin -1
+    ISO 8859-1
+    ISO  8859-15
+    KSC 5601 
+    Shift -JIS</t>
+  </si>
+  <si>
+    <t>System should display the list of character set options and allow to select  any options</t>
+  </si>
+  <si>
+    <t>Selecting the Target Catalog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+     </t>
+  </si>
+  <si>
+    <t>System should display the list of Target  catalog and allow to select  any options from the drop down.</t>
+  </si>
+  <si>
+    <t>Check for the uploaded file data in the respetive store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Check for the respective store where the uploaded file data is displaying or not
+     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the list of data which were uploaded in the  respective store </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the uploaded file data should not contains blank file </t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Check for the File which should not contains Blank file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should not allow to uplaod the blank file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the uploaded file data should  contains respective fileds which were displaying in the store </t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Check for the File which should  contains respective fields which were displaying  in the store</t>
+  </si>
+  <si>
+    <t>System should contains the respective field which were present in the Store as well as File upload</t>
+  </si>
+  <si>
+    <t>Check for the Save option</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Click on the Save Button</t>
+  </si>
+  <si>
+    <t>System should save the record and display the uploaded data in the respective store.</t>
+  </si>
+  <si>
+    <t>Check for the Close option</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Click on the Close Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should alert the user with prompting pop up window with 
+  Cancel
+  No 
+  Yes </t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Click on the Close Button
+11.Click on Cancel Button and select the option as Yes</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Click on the Close Button
+11.Click on Cancel Button and select the option as No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Click on the Close Button
+</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.Click on File --&gt; New --&gt; Catalog Upload option
+5.From the Main properties - File Name 
+6.Click on the File Browse option
+7.Select the XML/CSV File and cilck on Choose Button
+8.From the character set select any option from the drop down
+9.From the Target catalog select any store
+10.Click on the Close Button
+11.Click on Cancel Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecting the desired store from the drop down </t>
+  </si>
+  <si>
+    <t>System should display the list of  store from the desired Store management module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking  the desired store is present in the  drop down </t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.In the right pane of  the screen click on the drop down and check the list of store's list is displaying or not</t>
+  </si>
+  <si>
+    <t>System should display the list of  store from the drop down and it should allow to select the desired store</t>
+  </si>
+  <si>
+    <t>After selecting the desired store from the drop down and checking the screen</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.In the right pane of  the screen click on the drop down
+5.From the drop down select any of the store from the list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.In the right pane of  the screen click on the drop down
+5.From the drop down select any of the store from the list
+6.Once selected and check the store option is displaying in the left side navigation bar or not </t>
+  </si>
+  <si>
+    <t>System should allow to select the desired store and after the selection system should display the store option in the left side navigation bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the Store option and check the list of products displaying </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.In the right pane of  the screen click on the drop down
+5.From the drop down select any of the store from the list
+6.Once selected  , click the respective  store option and check the list of products pressent in the screen  </t>
+  </si>
+  <si>
+    <t>System should the details like 
+Sequence 
+Type 
+Code 
+Name 
+Display to Customers</t>
+  </si>
+  <si>
+    <t>Selecting the Extended Sites Catalog Asset Store  option from the File Menu</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the sequence field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the sequence field </t>
+  </si>
+  <si>
+    <t>System should display the details like 
+Sequence 
+Type 
+Code 
+Name 
+Display to Customers</t>
+  </si>
+  <si>
+    <t>System should display the details like 
+Sequence number for the product 
+either it would be high to low or vice verse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the Type  field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Type field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the Type  of the product 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the Store  field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Store field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the Store name for the mapped  product 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the Code  field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Code field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the Code number for the mapped  product 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the Name  field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Name field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the Name of the mapped  product 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check for the Display to Customers  field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Customers field </t>
+  </si>
+  <si>
+    <t>System should display the check box for the product is either selected to display to the customers or not</t>
+  </si>
+  <si>
+    <t>Check for the Display to Customers  field checked</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Customers field for checked option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the check box for the product is selected to display to the customers </t>
+  </si>
+  <si>
+    <t>Check for the Display to Customers  field  Unchecked</t>
+  </si>
+  <si>
+    <t>1.Navigate to the Management center tool application
+2.Click on the File Menu
+3.Click on Catalog Tool option
+4.From the file menu select Extended Sites Catalog Asset Store
+5.Check the Customers field for unchecked option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should display the check box for the product is unchecked and not display to the customers </t>
   </si>
 </sst>
 </file>
@@ -2425,7 +2883,7 @@
   <dimension ref="B3:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="35.6640625" defaultRowHeight="16"/>
@@ -2570,8 +3028,8 @@
       <c r="C15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>252</v>
+      <c r="D15" s="2">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="17">
@@ -2592,7 +3050,9 @@
       <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="17">
       <c r="B18" s="2">
@@ -2947,6 +3407,756 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9F1039-99A0-E249-86F6-B2359EE3408D}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="46" style="6" customWidth="1"/>
+    <col min="5" max="5" width="34" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="14.6640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="17">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="85">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="85">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="170">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="68">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="136">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="119">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="136">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="153">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="136">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="153">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="323">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="204">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="238">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="153">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="153">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="204">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="221">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="204">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="221">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="221">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="221">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF62A96F-EA56-BA47-B100-38CF0C5725C3}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="46" style="6" customWidth="1"/>
+    <col min="5" max="5" width="34" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="14.6640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="17">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="85">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="85">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="170">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="119">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="136">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="170">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="170">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF83F2C-A43D-0446-A98B-1B2510F1FC26}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="46" style="6" customWidth="1"/>
+    <col min="5" max="5" width="34" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="14.6640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="17">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="85">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="85">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="170">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="68">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="102">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="119">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="119">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="119">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="119">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="119">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="119">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="119">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="119">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>435</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D344A2F3-4BB2-9340-8D3D-DCECE8EC4799}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -3254,7 +4464,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
@@ -3484,8 +4694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361F6B21-A54C-2044-BCB4-6C9F869B5500}">
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A90"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>
@@ -4354,8 +5564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3ECF6A-593A-8D44-949C-82CE63425B7F}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A75"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16"/>

</xml_diff>